<commit_message>
Sensitivity to PV price, fix in HP cooling and HW start 1%
HP cooling EER=4
Scenario base: HWstorage start 1%

Sensitivity to PV price

Preparation of EE_NG price and start pf transport integration
</commit_message>
<xml_diff>
--- a/tesi_camilla/casi_MarioU/Sensitivity_EE_NG/PSV_prezzo_gas.xlsx
+++ b/tesi_camilla/casi_MarioU/Sensitivity_EE_NG/PSV_prezzo_gas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07445B3-3A9D-DE47-8088-D2EF842D67EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1472C6B7-A2C0-1C42-82AC-376D09A6B6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2253,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB35A66-6911-8241-B5BF-154DC12086A0}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2390,7 +2390,7 @@
         <v>27.648599999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:2">
       <c r="A17" s="30">
         <v>43040</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>28.74</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:2">
       <c r="A18" s="29">
         <v>43101</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>31.33</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:2">
       <c r="A19" s="30">
         <v>43191</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>28.441751783428572</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:2">
       <c r="A20" s="30">
         <v>43282</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>33.47</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:2">
       <c r="A21" s="30">
         <v>43405</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>36.666699999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:2">
       <c r="A22" s="29">
         <v>43466</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>37.287599999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:2">
       <c r="A23" s="30">
         <v>43556</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>29.723500000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:2">
       <c r="A24" s="30">
         <v>43647</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>25.25</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:2">
       <c r="A25" s="30">
         <v>43770</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>27.51</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:2">
       <c r="A26" s="29">
         <v>43831</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>28.33</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:2">
       <c r="A27" s="30">
         <v>43922</v>
       </c>
@@ -2478,23 +2478,15 @@
         <v>20.52</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:2">
       <c r="A28" s="30">
         <v>44013</v>
       </c>
       <c r="B28" s="1">
         <v>16.68</v>
       </c>
-      <c r="D28">
-        <f>B28/B60</f>
-        <v>0.40565188842141103</v>
-      </c>
-      <c r="E28">
-        <f>D28*0.55</f>
-        <v>0.2231085386317761</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="30">
         <v>44136</v>
       </c>
@@ -2502,7 +2494,7 @@
         <v>22.85</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:2">
       <c r="A30" s="29">
         <v>44197</v>
       </c>
@@ -2510,7 +2502,7 @@
         <v>25.64</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:2">
       <c r="A31" s="30">
         <v>44287</v>
       </c>
@@ -2518,7 +2510,7 @@
         <v>28.07</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:2">
       <c r="A32" s="30">
         <v>44378</v>
       </c>
@@ -2581,10 +2573,6 @@
       <c r="B39" s="1">
         <v>134.91999999999999</v>
       </c>
-      <c r="D39">
-        <f>B39/B60</f>
-        <v>3.2812082005885355</v>
-      </c>
       <c r="H39" s="33"/>
       <c r="I39" s="33"/>
     </row>
@@ -2781,14 +2769,6 @@
       </c>
       <c r="B60">
         <v>41.119</v>
-      </c>
-      <c r="D60">
-        <f>96.64/B60</f>
-        <v>2.3502517084559451</v>
-      </c>
-      <c r="E60">
-        <f>D60*0.55</f>
-        <v>1.29263843965077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>